<commit_message>
move table legends to freeze panel in excel sheets
</commit_message>
<xml_diff>
--- a/Tables/Supp Table 10 - HPOGOEnrichment.xlsx
+++ b/Tables/Supp Table 10 - HPOGOEnrichment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\CamocoManuscript\SuppTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\rob\Documents\CamocoManuscript\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28395" windowHeight="16560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28400" windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="104">
   <si>
     <t>bonferroni</t>
   </si>
@@ -328,6 +328,30 @@
   </si>
   <si>
     <t>GO Term Description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Element gene ontology enrichment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+HPO genes for each element were tested for enrichment among genes co-annotated for gene ontology (GO) terms (hypergeometric test). Bonferroni correction is included as a column, treating each GO term as an independent test.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -382,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -394,6 +418,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,94 +725,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.28515625" style="4"/>
+    <col min="8" max="8" width="10.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.26953125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>27</v>
-      </c>
-      <c r="E2" s="4">
-        <v>71</v>
-      </c>
-      <c r="F2" s="4">
-        <v>16953</v>
-      </c>
-      <c r="G2" s="4">
-        <v>5.6728053973108877E-3</v>
-      </c>
-      <c r="H2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -808,15 +819,15 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -828,27 +839,27 @@
         <v>27</v>
       </c>
       <c r="E4" s="4">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F4" s="4">
         <v>16953</v>
       </c>
       <c r="G4" s="4">
-        <v>8.0388701275701836E-3</v>
+        <v>5.6728053973108877E-3</v>
       </c>
       <c r="H4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -860,27 +871,27 @@
         <v>27</v>
       </c>
       <c r="E5" s="4">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F5" s="4">
         <v>16953</v>
       </c>
       <c r="G5" s="4">
-        <v>1.077507480471728E-2</v>
+        <v>8.0388701275701836E-3</v>
       </c>
       <c r="H5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -892,27 +903,27 @@
         <v>27</v>
       </c>
       <c r="E6" s="4">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F6" s="4">
         <v>16953</v>
       </c>
       <c r="G6" s="4">
-        <v>1.119522203754322E-2</v>
+        <v>1.077507480471728E-2</v>
       </c>
       <c r="H6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -924,27 +935,27 @@
         <v>27</v>
       </c>
       <c r="E7" s="4">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="F7" s="4">
         <v>16953</v>
       </c>
       <c r="G7" s="4">
-        <v>1.55379477799725E-2</v>
+        <v>1.119522203754322E-2</v>
       </c>
       <c r="H7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -956,59 +967,59 @@
         <v>27</v>
       </c>
       <c r="E8" s="4">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="F8" s="4">
         <v>16953</v>
       </c>
       <c r="G8" s="4">
-        <v>2.2173235469362819E-2</v>
+        <v>1.55379477799725E-2</v>
       </c>
       <c r="H8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4">
+        <v>145</v>
+      </c>
+      <c r="F9" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2.2173235469362819E-2</v>
+      </c>
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="4">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4">
-        <v>126</v>
-      </c>
-      <c r="E9" s="4">
-        <v>73</v>
-      </c>
-      <c r="F9" s="4">
-        <v>16953</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1.7091779210441919E-2</v>
-      </c>
-      <c r="H9" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
@@ -1032,15 +1043,15 @@
         <v>0</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -1064,15 +1075,15 @@
         <v>0</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>20</v>
@@ -1084,27 +1095,27 @@
         <v>126</v>
       </c>
       <c r="E12" s="4">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F12" s="4">
         <v>16953</v>
       </c>
       <c r="G12" s="4">
-        <v>1.967829043165515E-2</v>
+        <v>1.7091779210441919E-2</v>
       </c>
       <c r="H12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>20</v>
@@ -1116,27 +1127,27 @@
         <v>126</v>
       </c>
       <c r="E13" s="4">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F13" s="4">
         <v>16953</v>
       </c>
       <c r="G13" s="4">
-        <v>2.246909856215594E-2</v>
+        <v>1.967829043165515E-2</v>
       </c>
       <c r="H13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>20</v>
@@ -1148,27 +1159,27 @@
         <v>126</v>
       </c>
       <c r="E14" s="4">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F14" s="4">
         <v>16953</v>
       </c>
       <c r="G14" s="4">
-        <v>2.3941232602513171E-2</v>
+        <v>2.246909856215594E-2</v>
       </c>
       <c r="H14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>20</v>
@@ -1180,27 +1191,27 @@
         <v>126</v>
       </c>
       <c r="E15" s="4">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="F15" s="4">
         <v>16953</v>
       </c>
       <c r="G15" s="4">
-        <v>3.6605231913178451E-2</v>
+        <v>2.3941232602513171E-2</v>
       </c>
       <c r="H15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>20</v>
@@ -1212,27 +1223,27 @@
         <v>126</v>
       </c>
       <c r="E16" s="4">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" s="4">
         <v>16953</v>
       </c>
       <c r="G16" s="4">
-        <v>3.8507981690921782E-2</v>
+        <v>3.6605231913178451E-2</v>
       </c>
       <c r="H16" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
@@ -1256,15 +1267,15 @@
         <v>0</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
@@ -1276,27 +1287,27 @@
         <v>126</v>
       </c>
       <c r="E18" s="4">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F18" s="4">
         <v>16953</v>
       </c>
       <c r="G18" s="4">
-        <v>4.046037491780468E-2</v>
+        <v>3.8507981690921782E-2</v>
       </c>
       <c r="H18" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1320,15 +1331,15 @@
         <v>0</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
@@ -1340,27 +1351,27 @@
         <v>126</v>
       </c>
       <c r="E20" s="4">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F20" s="4">
         <v>16953</v>
       </c>
       <c r="G20" s="4">
-        <v>4.6612188526688449E-2</v>
+        <v>4.046037491780468E-2</v>
       </c>
       <c r="H20" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
@@ -1384,47 +1395,47 @@
         <v>0</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4">
         <v>3</v>
       </c>
       <c r="D22" s="4">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="E22" s="4">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="F22" s="4">
         <v>16953</v>
       </c>
       <c r="G22" s="4">
-        <v>1.609165342560546E-3</v>
+        <v>4.6612188526688449E-2</v>
       </c>
       <c r="H22" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>48</v>
@@ -1448,47 +1459,47 @@
         <v>0</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="4">
         <v>26</v>
       </c>
       <c r="E24" s="4">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F24" s="4">
         <v>16953</v>
       </c>
       <c r="G24" s="4">
-        <v>2.199552441429338E-2</v>
+        <v>1.609165342560546E-3</v>
       </c>
       <c r="H24" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>48</v>
@@ -1500,27 +1511,27 @@
         <v>26</v>
       </c>
       <c r="E25" s="4">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F25" s="4">
         <v>16953</v>
       </c>
       <c r="G25" s="4">
-        <v>2.5382508491766761E-2</v>
+        <v>2.199552441429338E-2</v>
       </c>
       <c r="H25" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>48</v>
@@ -1532,59 +1543,59 @@
         <v>26</v>
       </c>
       <c r="E26" s="4">
-        <v>209</v>
+        <v>162</v>
       </c>
       <c r="F26" s="4">
         <v>16953</v>
       </c>
       <c r="G26" s="4">
-        <v>4.0495073959185987E-2</v>
+        <v>2.5382508491766761E-2</v>
       </c>
       <c r="H26" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2</v>
+      </c>
+      <c r="D27" s="4">
+        <v>26</v>
+      </c>
+      <c r="E27" s="4">
+        <v>209</v>
+      </c>
+      <c r="F27" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G27" s="4">
+        <v>4.0495073959185987E-2</v>
+      </c>
+      <c r="H27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="4">
-        <v>4</v>
-      </c>
-      <c r="D27" s="4">
-        <v>76</v>
-      </c>
-      <c r="E27" s="4">
-        <v>79</v>
-      </c>
-      <c r="F27" s="4">
-        <v>16953</v>
-      </c>
-      <c r="G27" s="4">
-        <v>4.3443503542755932E-4</v>
-      </c>
-      <c r="H27" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>61</v>
@@ -1608,47 +1619,47 @@
         <v>0</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" s="4">
         <v>76</v>
       </c>
       <c r="E29" s="4">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4">
         <v>16953</v>
       </c>
       <c r="G29" s="4">
-        <v>8.4784937050692965E-3</v>
+        <v>4.3443503542755932E-4</v>
       </c>
       <c r="H29" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>61</v>
@@ -1672,15 +1683,15 @@
         <v>0</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>61</v>
@@ -1704,15 +1715,15 @@
         <v>0</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>61</v>
@@ -1724,27 +1735,27 @@
         <v>76</v>
       </c>
       <c r="E32" s="4">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="F32" s="4">
         <v>16953</v>
       </c>
       <c r="G32" s="4">
-        <v>3.0611450596851719E-2</v>
+        <v>8.4784937050692965E-3</v>
       </c>
       <c r="H32" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>61</v>
@@ -1756,27 +1767,27 @@
         <v>76</v>
       </c>
       <c r="E33" s="4">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F33" s="4">
         <v>16953</v>
       </c>
       <c r="G33" s="4">
-        <v>3.8356877112621812E-2</v>
+        <v>3.0611450596851719E-2</v>
       </c>
       <c r="H33" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>61</v>
@@ -1788,27 +1799,27 @@
         <v>76</v>
       </c>
       <c r="E34" s="4">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F34" s="4">
         <v>16953</v>
       </c>
       <c r="G34" s="4">
-        <v>4.2480743208483648E-2</v>
+        <v>3.8356877112621812E-2</v>
       </c>
       <c r="H34" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>61</v>
@@ -1820,59 +1831,59 @@
         <v>76</v>
       </c>
       <c r="E35" s="4">
+        <v>73</v>
+      </c>
+      <c r="F35" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.2480743208483648E-2</v>
+      </c>
+      <c r="H35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="4">
-        <v>16953</v>
-      </c>
-      <c r="G35" s="4">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4">
+        <v>76</v>
+      </c>
+      <c r="E36" s="4">
+        <v>77</v>
+      </c>
+      <c r="F36" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G36" s="4">
         <v>4.6762689241433571E-2</v>
       </c>
-      <c r="H35" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="4" t="s">
+      <c r="H36" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="4">
-        <v>4</v>
-      </c>
-      <c r="D36" s="4">
-        <v>58</v>
-      </c>
-      <c r="E36" s="4">
-        <v>237</v>
-      </c>
-      <c r="F36" s="4">
-        <v>16953</v>
-      </c>
-      <c r="G36" s="4">
-        <v>8.7582899104470743E-3</v>
-      </c>
-      <c r="H36" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>85</v>
@@ -1884,59 +1895,59 @@
         <v>58</v>
       </c>
       <c r="E37" s="4">
-        <v>279</v>
+        <v>237</v>
       </c>
       <c r="F37" s="4">
         <v>16953</v>
       </c>
       <c r="G37" s="4">
-        <v>1.5197282616416931E-2</v>
+        <v>8.7582899104470743E-3</v>
       </c>
       <c r="H37" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D38" s="4">
         <v>58</v>
       </c>
       <c r="E38" s="4">
-        <v>55</v>
+        <v>279</v>
       </c>
       <c r="F38" s="4">
         <v>16953</v>
       </c>
       <c r="G38" s="4">
-        <v>1.520972332695607E-2</v>
+        <v>1.5197282616416931E-2</v>
       </c>
       <c r="H38" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>85</v>
@@ -1948,27 +1959,27 @@
         <v>58</v>
       </c>
       <c r="E39" s="4">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="F39" s="4">
         <v>16953</v>
       </c>
       <c r="G39" s="4">
-        <v>2.5884258965599649E-2</v>
+        <v>1.520972332695607E-2</v>
       </c>
       <c r="H39" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>85</v>
@@ -1992,15 +2003,15 @@
         <v>0</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>85</v>
@@ -2024,15 +2035,15 @@
         <v>0</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>85</v>
@@ -2044,27 +2055,27 @@
         <v>58</v>
       </c>
       <c r="E42" s="4">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F42" s="4">
         <v>16953</v>
       </c>
       <c r="G42" s="4">
-        <v>2.8570682771111529E-2</v>
+        <v>2.5884258965599649E-2</v>
       </c>
       <c r="H42" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>85</v>
@@ -2076,27 +2087,27 @@
         <v>58</v>
       </c>
       <c r="E43" s="4">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F43" s="4">
         <v>16953</v>
       </c>
       <c r="G43" s="4">
-        <v>3.1363966425433792E-2</v>
+        <v>2.8570682771111529E-2</v>
       </c>
       <c r="H43" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>85</v>
@@ -2108,91 +2119,91 @@
         <v>58</v>
       </c>
       <c r="E44" s="4">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F44" s="4">
         <v>16953</v>
       </c>
       <c r="G44" s="4">
-        <v>3.2799646670696757E-2</v>
+        <v>3.1363966425433792E-2</v>
       </c>
       <c r="H44" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" s="4">
         <v>58</v>
       </c>
       <c r="E45" s="4">
-        <v>209</v>
+        <v>83</v>
       </c>
       <c r="F45" s="4">
         <v>16953</v>
       </c>
       <c r="G45" s="4">
-        <v>3.4724782031211592E-2</v>
+        <v>3.2799646670696757E-2</v>
       </c>
       <c r="H45" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C46" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46" s="4">
         <v>58</v>
       </c>
       <c r="E46" s="4">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="F46" s="4">
         <v>16953</v>
       </c>
       <c r="G46" s="4">
-        <v>4.4352129898147692E-2</v>
+        <v>3.4724782031211592E-2</v>
       </c>
       <c r="H46" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>85</v>
@@ -2204,27 +2215,27 @@
         <v>58</v>
       </c>
       <c r="E47" s="4">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F47" s="4">
         <v>16953</v>
       </c>
       <c r="G47" s="4">
-        <v>4.5991879361038081E-2</v>
+        <v>4.4352129898147692E-2</v>
       </c>
       <c r="H47" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>85</v>
@@ -2248,15 +2259,15 @@
         <v>0</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>85</v>
@@ -2268,27 +2279,27 @@
         <v>58</v>
       </c>
       <c r="E49" s="4">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F49" s="4">
         <v>16953</v>
       </c>
       <c r="G49" s="4">
-        <v>4.7653823433669869E-2</v>
+        <v>4.5991879361038081E-2</v>
       </c>
       <c r="H49" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>85</v>
@@ -2312,13 +2323,48 @@
         <v>0</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="4">
+        <v>2</v>
+      </c>
+      <c r="D51" s="4">
+        <v>58</v>
+      </c>
+      <c r="E51" s="4">
+        <v>102</v>
+      </c>
+      <c r="F51" s="4">
+        <v>16953</v>
+      </c>
+      <c r="G51" s="4">
+        <v>4.7653823433669869E-2</v>
+      </c>
+      <c r="H51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
check sig figs on all tables
</commit_message>
<xml_diff>
--- a/Tables/Supp Table 10 - HPOGOEnrichment.xlsx
+++ b/Tables/Supp Table 10 - HPOGOEnrichment.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28400" windowHeight="16560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28395" windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -419,9 +419,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,39 +731,39 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.26953125" style="4"/>
+    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.28515625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
@@ -793,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -813,7 +815,7 @@
         <v>16953</v>
       </c>
       <c r="G3" s="4">
-        <v>5.6728053973108877E-3</v>
+        <v>5.6699999999999997E-3</v>
       </c>
       <c r="H3" s="4" t="b">
         <v>0</v>
@@ -825,7 +827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -845,7 +847,7 @@
         <v>16953</v>
       </c>
       <c r="G4" s="4">
-        <v>5.6728053973108877E-3</v>
+        <v>5.6699999999999997E-3</v>
       </c>
       <c r="H4" s="4" t="b">
         <v>0</v>
@@ -857,7 +859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -877,7 +879,7 @@
         <v>16953</v>
       </c>
       <c r="G5" s="4">
-        <v>8.0388701275701836E-3</v>
+        <v>8.0400000000000003E-3</v>
       </c>
       <c r="H5" s="4" t="b">
         <v>0</v>
@@ -889,7 +891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -909,7 +911,7 @@
         <v>16953</v>
       </c>
       <c r="G6" s="4">
-        <v>1.077507480471728E-2</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="H6" s="4" t="b">
         <v>0</v>
@@ -921,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -941,7 +943,7 @@
         <v>16953</v>
       </c>
       <c r="G7" s="4">
-        <v>1.119522203754322E-2</v>
+        <v>1.12E-2</v>
       </c>
       <c r="H7" s="4" t="b">
         <v>0</v>
@@ -953,7 +955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -973,7 +975,7 @@
         <v>16953</v>
       </c>
       <c r="G8" s="4">
-        <v>1.55379477799725E-2</v>
+        <v>1.55E-2</v>
       </c>
       <c r="H8" s="4" t="b">
         <v>0</v>
@@ -985,7 +987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1005,7 +1007,7 @@
         <v>16953</v>
       </c>
       <c r="G9" s="4">
-        <v>2.2173235469362819E-2</v>
+        <v>2.2200000000000001E-2</v>
       </c>
       <c r="H9" s="4" t="b">
         <v>0</v>
@@ -1017,7 +1019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>16953</v>
       </c>
       <c r="G10" s="4">
-        <v>1.7091779210441919E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="H10" s="4" t="b">
         <v>0</v>
@@ -1049,7 +1051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1069,7 +1071,7 @@
         <v>16953</v>
       </c>
       <c r="G11" s="4">
-        <v>1.7091779210441919E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="H11" s="4" t="b">
         <v>0</v>
@@ -1081,7 +1083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -1101,7 +1103,7 @@
         <v>16953</v>
       </c>
       <c r="G12" s="4">
-        <v>1.7091779210441919E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="H12" s="4" t="b">
         <v>0</v>
@@ -1113,7 +1115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>16953</v>
       </c>
       <c r="G13" s="4">
-        <v>1.967829043165515E-2</v>
+        <v>1.9699999999999999E-2</v>
       </c>
       <c r="H13" s="4" t="b">
         <v>0</v>
@@ -1145,7 +1147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>16953</v>
       </c>
       <c r="G14" s="4">
-        <v>2.246909856215594E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="H14" s="4" t="b">
         <v>0</v>
@@ -1177,7 +1179,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1197,7 +1199,7 @@
         <v>16953</v>
       </c>
       <c r="G15" s="4">
-        <v>2.3941232602513171E-2</v>
+        <v>2.3900000000000001E-2</v>
       </c>
       <c r="H15" s="4" t="b">
         <v>0</v>
@@ -1209,7 +1211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -1229,7 +1231,7 @@
         <v>16953</v>
       </c>
       <c r="G16" s="4">
-        <v>3.6605231913178451E-2</v>
+        <v>3.6600000000000001E-2</v>
       </c>
       <c r="H16" s="4" t="b">
         <v>0</v>
@@ -1241,7 +1243,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -1261,7 +1263,7 @@
         <v>16953</v>
       </c>
       <c r="G17" s="4">
-        <v>3.8507981690921782E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="H17" s="4" t="b">
         <v>0</v>
@@ -1273,7 +1275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -1293,7 +1295,7 @@
         <v>16953</v>
       </c>
       <c r="G18" s="4">
-        <v>3.8507981690921782E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="H18" s="4" t="b">
         <v>0</v>
@@ -1305,7 +1307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>16953</v>
       </c>
       <c r="G19" s="4">
-        <v>4.046037491780468E-2</v>
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="H19" s="4" t="b">
         <v>0</v>
@@ -1337,7 +1339,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
@@ -1357,7 +1359,7 @@
         <v>16953</v>
       </c>
       <c r="G20" s="4">
-        <v>4.046037491780468E-2</v>
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="H20" s="4" t="b">
         <v>0</v>
@@ -1369,7 +1371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>16953</v>
       </c>
       <c r="G21" s="4">
-        <v>4.6612188526688449E-2</v>
+        <v>4.6600000000000003E-2</v>
       </c>
       <c r="H21" s="4" t="b">
         <v>0</v>
@@ -1401,7 +1403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>16953</v>
       </c>
       <c r="G22" s="4">
-        <v>4.6612188526688449E-2</v>
+        <v>4.6600000000000003E-2</v>
       </c>
       <c r="H22" s="4" t="b">
         <v>0</v>
@@ -1433,7 +1435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1453,7 +1455,7 @@
         <v>16953</v>
       </c>
       <c r="G23" s="4">
-        <v>1.609165342560546E-3</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="H23" s="4" t="b">
         <v>0</v>
@@ -1465,7 +1467,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
@@ -1485,7 +1487,7 @@
         <v>16953</v>
       </c>
       <c r="G24" s="4">
-        <v>1.609165342560546E-3</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="H24" s="4" t="b">
         <v>0</v>
@@ -1497,7 +1499,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -1517,7 +1519,7 @@
         <v>16953</v>
       </c>
       <c r="G25" s="4">
-        <v>2.199552441429338E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H25" s="4" t="b">
         <v>0</v>
@@ -1529,7 +1531,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1549,7 +1551,7 @@
         <v>16953</v>
       </c>
       <c r="G26" s="4">
-        <v>2.5382508491766761E-2</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="H26" s="4" t="b">
         <v>0</v>
@@ -1561,7 +1563,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -1581,7 +1583,7 @@
         <v>16953</v>
       </c>
       <c r="G27" s="4">
-        <v>4.0495073959185987E-2</v>
+        <v>4.0500000000000001E-2</v>
       </c>
       <c r="H27" s="4" t="b">
         <v>0</v>
@@ -1593,7 +1595,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>60</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>16953</v>
       </c>
       <c r="G28" s="4">
-        <v>4.3443503542755932E-4</v>
+        <v>4.3399999999999998E-4</v>
       </c>
       <c r="H28" s="4" t="b">
         <v>0</v>
@@ -1625,7 +1627,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
@@ -1645,7 +1647,7 @@
         <v>16953</v>
       </c>
       <c r="G29" s="4">
-        <v>4.3443503542755932E-4</v>
+        <v>4.3399999999999998E-4</v>
       </c>
       <c r="H29" s="4" t="b">
         <v>0</v>
@@ -1657,7 +1659,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -1677,7 +1679,7 @@
         <v>16953</v>
       </c>
       <c r="G30" s="4">
-        <v>8.4784937050692965E-3</v>
+        <v>8.4799999999999997E-3</v>
       </c>
       <c r="H30" s="4" t="b">
         <v>0</v>
@@ -1689,7 +1691,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>69</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>16953</v>
       </c>
       <c r="G31" s="4">
-        <v>8.4784937050692965E-3</v>
+        <v>8.4799999999999997E-3</v>
       </c>
       <c r="H31" s="4" t="b">
         <v>0</v>
@@ -1721,7 +1723,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>71</v>
       </c>
@@ -1741,7 +1743,7 @@
         <v>16953</v>
       </c>
       <c r="G32" s="4">
-        <v>8.4784937050692965E-3</v>
+        <v>8.4799999999999997E-3</v>
       </c>
       <c r="H32" s="4" t="b">
         <v>0</v>
@@ -1753,7 +1755,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>73</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>16953</v>
       </c>
       <c r="G33" s="4">
-        <v>3.0611450596851719E-2</v>
+        <v>3.0599999999999999E-2</v>
       </c>
       <c r="H33" s="4" t="b">
         <v>0</v>
@@ -1785,7 +1787,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>76</v>
       </c>
@@ -1805,7 +1807,7 @@
         <v>16953</v>
       </c>
       <c r="G34" s="4">
-        <v>3.8356877112621812E-2</v>
+        <v>3.8399999999999997E-2</v>
       </c>
       <c r="H34" s="4" t="b">
         <v>0</v>
@@ -1817,7 +1819,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>79</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>16953</v>
       </c>
       <c r="G35" s="4">
-        <v>4.2480743208483648E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="H35" s="4" t="b">
         <v>0</v>
@@ -1849,7 +1851,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>81</v>
       </c>
@@ -1869,7 +1871,7 @@
         <v>16953</v>
       </c>
       <c r="G36" s="4">
-        <v>4.6762689241433571E-2</v>
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="H36" s="4" t="b">
         <v>0</v>
@@ -1881,7 +1883,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>16953</v>
       </c>
       <c r="G37" s="4">
-        <v>8.7582899104470743E-3</v>
+        <v>8.7600000000000004E-3</v>
       </c>
       <c r="H37" s="4" t="b">
         <v>0</v>
@@ -1913,7 +1915,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>16953</v>
       </c>
       <c r="G38" s="4">
-        <v>1.5197282616416931E-2</v>
+        <v>1.52E-2</v>
       </c>
       <c r="H38" s="4" t="b">
         <v>0</v>
@@ -1945,7 +1947,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>91</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>16953</v>
       </c>
       <c r="G39" s="4">
-        <v>1.520972332695607E-2</v>
+        <v>1.52E-2</v>
       </c>
       <c r="H39" s="4" t="b">
         <v>0</v>
@@ -1977,7 +1979,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>19</v>
       </c>
@@ -1997,7 +1999,7 @@
         <v>16953</v>
       </c>
       <c r="G40" s="4">
-        <v>2.5884258965599649E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="H40" s="4" t="b">
         <v>0</v>
@@ -2009,7 +2011,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
@@ -2029,7 +2031,7 @@
         <v>16953</v>
       </c>
       <c r="G41" s="4">
-        <v>2.5884258965599649E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="H41" s="4" t="b">
         <v>0</v>
@@ -2041,7 +2043,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>25</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>16953</v>
       </c>
       <c r="G42" s="4">
-        <v>2.5884258965599649E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="H42" s="4" t="b">
         <v>0</v>
@@ -2073,7 +2075,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
@@ -2093,7 +2095,7 @@
         <v>16953</v>
       </c>
       <c r="G43" s="4">
-        <v>2.8570682771111529E-2</v>
+        <v>2.86E-2</v>
       </c>
       <c r="H43" s="4" t="b">
         <v>0</v>
@@ -2105,7 +2107,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>29</v>
       </c>
@@ -2125,7 +2127,7 @@
         <v>16953</v>
       </c>
       <c r="G44" s="4">
-        <v>3.1363966425433792E-2</v>
+        <v>3.1399999999999997E-2</v>
       </c>
       <c r="H44" s="4" t="b">
         <v>0</v>
@@ -2137,7 +2139,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>31</v>
       </c>
@@ -2157,7 +2159,7 @@
         <v>16953</v>
       </c>
       <c r="G45" s="4">
-        <v>3.2799646670696757E-2</v>
+        <v>3.2800000000000003E-2</v>
       </c>
       <c r="H45" s="4" t="b">
         <v>0</v>
@@ -2169,7 +2171,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>16953</v>
       </c>
       <c r="G46" s="4">
-        <v>3.4724782031211592E-2</v>
+        <v>3.4700000000000002E-2</v>
       </c>
       <c r="H46" s="4" t="b">
         <v>0</v>
@@ -2201,7 +2203,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>33</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>16953</v>
       </c>
       <c r="G47" s="4">
-        <v>4.4352129898147692E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="H47" s="4" t="b">
         <v>0</v>
@@ -2233,7 +2235,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>35</v>
       </c>
@@ -2253,7 +2255,7 @@
         <v>16953</v>
       </c>
       <c r="G48" s="4">
-        <v>4.5991879361038081E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H48" s="4" t="b">
         <v>0</v>
@@ -2265,7 +2267,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>37</v>
       </c>
@@ -2285,7 +2287,7 @@
         <v>16953</v>
       </c>
       <c r="G49" s="4">
-        <v>4.5991879361038081E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H49" s="4" t="b">
         <v>0</v>
@@ -2297,7 +2299,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>39</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>16953</v>
       </c>
       <c r="G50" s="4">
-        <v>4.7653823433669869E-2</v>
+        <v>4.7699999999999999E-2</v>
       </c>
       <c r="H50" s="4" t="b">
         <v>0</v>
@@ -2329,7 +2331,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>41</v>
       </c>
@@ -2349,7 +2351,7 @@
         <v>16953</v>
       </c>
       <c r="G51" s="4">
-        <v>4.7653823433669869E-2</v>
+        <v>4.7699999999999999E-2</v>
       </c>
       <c r="H51" s="4" t="b">
         <v>0</v>

</xml_diff>